<commit_message>
Treffen mit Noe 28.02.2024
Notizen. Update des Zeitplans. Termine für neue Absprachetrefffen
</commit_message>
<xml_diff>
--- a/Schachroboter_Zeitplan.xlsx
+++ b/Schachroboter_Zeitplan.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9886F9-57BF-4D64-9EDA-DE8BD24D3202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB18C0D-2725-4E40-9204-A0EB4992E025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="415" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-4790" windowWidth="38620" windowHeight="21100" tabRatio="415" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="12" r:id="rId1"/>
@@ -3183,7 +3183,7 @@
       </c>
       <c r="C6" s="80" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">IFERROR(IF(MIN(Meilensteine4352[Start])=0,TODAY(),B11(Meilensteine4352[Start])),TODAY())</f>
-        <v>45348</v>
+        <v>45350</v>
       </c>
       <c r="D6" s="81"/>
       <c r="E6" s="75"/>
@@ -3286,227 +3286,227 @@
       <c r="H7" s="83"/>
       <c r="I7" s="98">
         <f ca="1">IFERROR(Projekt_Start+Scrollschrittweite,TODAY())</f>
-        <v>45349</v>
+        <v>45351</v>
       </c>
       <c r="J7" s="99">
         <f ca="1">I7+1</f>
-        <v>45350</v>
+        <v>45352</v>
       </c>
       <c r="K7" s="99">
         <f t="shared" ref="K7:AX7" ca="1" si="0">J7+1</f>
-        <v>45351</v>
+        <v>45353</v>
       </c>
       <c r="L7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45352</v>
+        <v>45354</v>
       </c>
       <c r="M7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45353</v>
+        <v>45355</v>
       </c>
       <c r="N7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45354</v>
+        <v>45356</v>
       </c>
       <c r="O7" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>45355</v>
+        <v>45357</v>
       </c>
       <c r="P7" s="99">
         <f ca="1">O7+1</f>
-        <v>45356</v>
+        <v>45358</v>
       </c>
       <c r="Q7" s="99">
         <f ca="1">P7+1</f>
-        <v>45357</v>
+        <v>45359</v>
       </c>
       <c r="R7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45358</v>
+        <v>45360</v>
       </c>
       <c r="S7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45359</v>
+        <v>45361</v>
       </c>
       <c r="T7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45360</v>
+        <v>45362</v>
       </c>
       <c r="U7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="V7" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>45362</v>
+        <v>45364</v>
       </c>
       <c r="W7" s="99">
         <f ca="1">V7+1</f>
-        <v>45363</v>
+        <v>45365</v>
       </c>
       <c r="X7" s="99">
         <f ca="1">W7+1</f>
-        <v>45364</v>
+        <v>45366</v>
       </c>
       <c r="Y7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45365</v>
+        <v>45367</v>
       </c>
       <c r="Z7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45366</v>
+        <v>45368</v>
       </c>
       <c r="AA7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45367</v>
+        <v>45369</v>
       </c>
       <c r="AB7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45368</v>
+        <v>45370</v>
       </c>
       <c r="AC7" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>45369</v>
+        <v>45371</v>
       </c>
       <c r="AD7" s="99">
         <f ca="1">AC7+1</f>
-        <v>45370</v>
+        <v>45372</v>
       </c>
       <c r="AE7" s="99">
         <f ca="1">AD7+1</f>
-        <v>45371</v>
+        <v>45373</v>
       </c>
       <c r="AF7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45372</v>
+        <v>45374</v>
       </c>
       <c r="AG7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45373</v>
+        <v>45375</v>
       </c>
       <c r="AH7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45374</v>
+        <v>45376</v>
       </c>
       <c r="AI7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45375</v>
+        <v>45377</v>
       </c>
       <c r="AJ7" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>45376</v>
+        <v>45378</v>
       </c>
       <c r="AK7" s="99">
         <f ca="1">AJ7+1</f>
-        <v>45377</v>
+        <v>45379</v>
       </c>
       <c r="AL7" s="99">
         <f ca="1">AK7+1</f>
-        <v>45378</v>
+        <v>45380</v>
       </c>
       <c r="AM7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45379</v>
+        <v>45381</v>
       </c>
       <c r="AN7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45380</v>
+        <v>45382</v>
       </c>
       <c r="AO7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45381</v>
+        <v>45383</v>
       </c>
       <c r="AP7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45382</v>
+        <v>45384</v>
       </c>
       <c r="AQ7" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>45383</v>
+        <v>45385</v>
       </c>
       <c r="AR7" s="99">
         <f ca="1">AQ7+1</f>
-        <v>45384</v>
+        <v>45386</v>
       </c>
       <c r="AS7" s="99">
         <f ca="1">AR7+1</f>
-        <v>45385</v>
+        <v>45387</v>
       </c>
       <c r="AT7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45386</v>
+        <v>45388</v>
       </c>
       <c r="AU7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45387</v>
+        <v>45389</v>
       </c>
       <c r="AV7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45388</v>
+        <v>45390</v>
       </c>
       <c r="AW7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45389</v>
+        <v>45391</v>
       </c>
       <c r="AX7" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>45390</v>
+        <v>45392</v>
       </c>
       <c r="AY7" s="99">
         <f ca="1">AX7+1</f>
-        <v>45391</v>
+        <v>45393</v>
       </c>
       <c r="AZ7" s="99">
         <f ca="1">AY7+1</f>
-        <v>45392</v>
+        <v>45394</v>
       </c>
       <c r="BA7" s="99">
         <f t="shared" ref="BA7:BE7" ca="1" si="1">AZ7+1</f>
-        <v>45393</v>
+        <v>45395</v>
       </c>
       <c r="BB7" s="99">
         <f t="shared" ca="1" si="1"/>
-        <v>45394</v>
+        <v>45396</v>
       </c>
       <c r="BC7" s="99">
         <f t="shared" ca="1" si="1"/>
-        <v>45395</v>
+        <v>45397</v>
       </c>
       <c r="BD7" s="99">
         <f t="shared" ca="1" si="1"/>
-        <v>45396</v>
+        <v>45398</v>
       </c>
       <c r="BE7" s="100">
         <f t="shared" ca="1" si="1"/>
-        <v>45397</v>
+        <v>45399</v>
       </c>
       <c r="BF7" s="99">
         <f ca="1">BE7+1</f>
-        <v>45398</v>
+        <v>45400</v>
       </c>
       <c r="BG7" s="99">
         <f ca="1">BF7+1</f>
-        <v>45399</v>
+        <v>45401</v>
       </c>
       <c r="BH7" s="99">
         <f t="shared" ref="BH7:BL7" ca="1" si="2">BG7+1</f>
-        <v>45400</v>
+        <v>45402</v>
       </c>
       <c r="BI7" s="99">
         <f t="shared" ca="1" si="2"/>
-        <v>45401</v>
+        <v>45403</v>
       </c>
       <c r="BJ7" s="99">
         <f t="shared" ca="1" si="2"/>
-        <v>45402</v>
+        <v>45404</v>
       </c>
       <c r="BK7" s="99">
         <f t="shared" ca="1" si="2"/>
-        <v>45403</v>
+        <v>45405</v>
       </c>
       <c r="BL7" s="100">
         <f t="shared" ca="1" si="2"/>
-        <v>45404</v>
+        <v>45406</v>
       </c>
     </row>
     <row r="8" spans="1:68" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3604,23 +3604,23 @@
       </c>
       <c r="J9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="K9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="L9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="M9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="N9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="O9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3632,23 +3632,23 @@
       </c>
       <c r="Q9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="R9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="S9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="T9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="U9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="V9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3660,23 +3660,23 @@
       </c>
       <c r="X9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="Y9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="Z9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="AA9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="AB9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="AC9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3688,23 +3688,23 @@
       </c>
       <c r="AE9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="AF9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="AG9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="AH9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="AI9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="AJ9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3716,23 +3716,23 @@
       </c>
       <c r="AL9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="AM9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="AN9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="AO9" s="106" t="str">
         <f t="shared" ref="AO9:BL9" ca="1" si="4">LEFT(TEXT(AO7,"TTT"),1)</f>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="AP9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="AQ9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -3744,23 +3744,23 @@
       </c>
       <c r="AS9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="AT9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="AU9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="AV9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="AW9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="AX9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -3772,23 +3772,23 @@
       </c>
       <c r="AZ9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="BA9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="BB9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="BC9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="BD9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="BE9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -3800,23 +3800,23 @@
       </c>
       <c r="BG9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="BH9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="BI9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="BJ9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="BK9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="BL9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -4140,7 +4140,7 @@
       </c>
       <c r="F12" s="61">
         <f ca="1">TODAY()</f>
-        <v>45348</v>
+        <v>45350</v>
       </c>
       <c r="G12" s="62">
         <v>3</v>
@@ -4383,7 +4383,7 @@
       <c r="E13" s="60"/>
       <c r="F13" s="61">
         <f ca="1">TODAY()+5</f>
-        <v>45353</v>
+        <v>45355</v>
       </c>
       <c r="G13" s="62">
         <v>1</v>
@@ -4628,7 +4628,7 @@
       </c>
       <c r="F14" s="61">
         <f ca="1">F12-3</f>
-        <v>45345</v>
+        <v>45347</v>
       </c>
       <c r="G14" s="62">
         <v>10</v>
@@ -4871,7 +4871,7 @@
       <c r="E15" s="60"/>
       <c r="F15" s="61">
         <f ca="1">F12+20</f>
-        <v>45368</v>
+        <v>45370</v>
       </c>
       <c r="G15" s="62">
         <v>1</v>
@@ -5116,7 +5116,7 @@
       </c>
       <c r="F16" s="61">
         <f ca="1">F12+6</f>
-        <v>45354</v>
+        <v>45356</v>
       </c>
       <c r="G16" s="62">
         <v>6</v>
@@ -5597,7 +5597,7 @@
       </c>
       <c r="F18" s="61">
         <f ca="1">F12+6</f>
-        <v>45354</v>
+        <v>45356</v>
       </c>
       <c r="G18" s="62">
         <v>13</v>
@@ -5842,7 +5842,7 @@
       </c>
       <c r="F19" s="61">
         <f ca="1">F18+2</f>
-        <v>45356</v>
+        <v>45358</v>
       </c>
       <c r="G19" s="62">
         <v>9</v>
@@ -6087,7 +6087,7 @@
       </c>
       <c r="F20" s="61">
         <f ca="1">F19+5</f>
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="G20" s="62">
         <v>11</v>
@@ -6330,7 +6330,7 @@
       <c r="E21" s="60"/>
       <c r="F21" s="61">
         <f ca="1">F20+2</f>
-        <v>45363</v>
+        <v>45365</v>
       </c>
       <c r="G21" s="62">
         <v>1</v>
@@ -6571,7 +6571,7 @@
       <c r="E22" s="60"/>
       <c r="F22" s="61">
         <f ca="1">F21+1</f>
-        <v>45364</v>
+        <v>45366</v>
       </c>
       <c r="G22" s="62">
         <v>24</v>
@@ -7050,7 +7050,7 @@
       <c r="E24" s="60"/>
       <c r="F24" s="61">
         <f ca="1">F12+15</f>
-        <v>45363</v>
+        <v>45365</v>
       </c>
       <c r="G24" s="62">
         <v>4</v>
@@ -7293,7 +7293,7 @@
       <c r="E25" s="60"/>
       <c r="F25" s="61">
         <f ca="1">F24+3</f>
-        <v>45366</v>
+        <v>45368</v>
       </c>
       <c r="G25" s="62">
         <v>14</v>
@@ -7536,7 +7536,7 @@
       <c r="E26" s="60"/>
       <c r="F26" s="61">
         <f ca="1">F25+15</f>
-        <v>45381</v>
+        <v>45383</v>
       </c>
       <c r="G26" s="62">
         <v>6</v>
@@ -7779,7 +7779,7 @@
       <c r="E27" s="60"/>
       <c r="F27" s="61">
         <f ca="1">F21+22</f>
-        <v>45385</v>
+        <v>45387</v>
       </c>
       <c r="G27" s="62">
         <v>3</v>
@@ -8022,7 +8022,7 @@
       <c r="E28" s="60"/>
       <c r="F28" s="61">
         <f ca="1">F16</f>
-        <v>45354</v>
+        <v>45356</v>
       </c>
       <c r="G28" s="62">
         <v>19</v>
@@ -8499,7 +8499,7 @@
       <c r="E30" s="60"/>
       <c r="F30" s="61">
         <f ca="1">F27+3</f>
-        <v>45388</v>
+        <v>45390</v>
       </c>
       <c r="G30" s="62">
         <v>15</v>
@@ -8740,7 +8740,7 @@
       <c r="E31" s="60"/>
       <c r="F31" s="61">
         <f ca="1">F30+14</f>
-        <v>45402</v>
+        <v>45404</v>
       </c>
       <c r="G31" s="62">
         <v>5</v>
@@ -8983,7 +8983,7 @@
       <c r="E32" s="60"/>
       <c r="F32" s="61">
         <f ca="1">F31+42</f>
-        <v>45444</v>
+        <v>45446</v>
       </c>
       <c r="G32" s="62">
         <v>1</v>
@@ -10472,7 +10472,7 @@
       </c>
       <c r="C6" s="34" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">IFERROR(IF(MIN(Meilensteine435[Start])=0,TODAY(),B11(Meilensteine435[Start])),TODAY())</f>
-        <v>45348</v>
+        <v>45350</v>
       </c>
       <c r="D6" s="53"/>
       <c r="E6" s="32"/>
@@ -10576,227 +10576,227 @@
       <c r="H7" s="29"/>
       <c r="I7" s="96">
         <f ca="1">IFERROR(Projekt_Start+Scrollschrittweite,TODAY())</f>
-        <v>45349</v>
+        <v>45351</v>
       </c>
       <c r="J7" s="17">
         <f ca="1">I7+1</f>
-        <v>45350</v>
+        <v>45352</v>
       </c>
       <c r="K7" s="17">
         <f t="shared" ref="K7:AX7" ca="1" si="0">J7+1</f>
-        <v>45351</v>
+        <v>45353</v>
       </c>
       <c r="L7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45352</v>
+        <v>45354</v>
       </c>
       <c r="M7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45353</v>
+        <v>45355</v>
       </c>
       <c r="N7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45354</v>
+        <v>45356</v>
       </c>
       <c r="O7" s="64">
         <f t="shared" ca="1" si="0"/>
-        <v>45355</v>
+        <v>45357</v>
       </c>
       <c r="P7" s="17">
         <f ca="1">O7+1</f>
-        <v>45356</v>
+        <v>45358</v>
       </c>
       <c r="Q7" s="17">
         <f ca="1">P7+1</f>
-        <v>45357</v>
+        <v>45359</v>
       </c>
       <c r="R7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45358</v>
+        <v>45360</v>
       </c>
       <c r="S7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45359</v>
+        <v>45361</v>
       </c>
       <c r="T7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45360</v>
+        <v>45362</v>
       </c>
       <c r="U7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="V7" s="64">
         <f t="shared" ca="1" si="0"/>
-        <v>45362</v>
+        <v>45364</v>
       </c>
       <c r="W7" s="17">
         <f ca="1">V7+1</f>
-        <v>45363</v>
+        <v>45365</v>
       </c>
       <c r="X7" s="17">
         <f ca="1">W7+1</f>
-        <v>45364</v>
+        <v>45366</v>
       </c>
       <c r="Y7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45365</v>
+        <v>45367</v>
       </c>
       <c r="Z7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45366</v>
+        <v>45368</v>
       </c>
       <c r="AA7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45367</v>
+        <v>45369</v>
       </c>
       <c r="AB7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45368</v>
+        <v>45370</v>
       </c>
       <c r="AC7" s="64">
         <f t="shared" ca="1" si="0"/>
-        <v>45369</v>
+        <v>45371</v>
       </c>
       <c r="AD7" s="17">
         <f ca="1">AC7+1</f>
-        <v>45370</v>
+        <v>45372</v>
       </c>
       <c r="AE7" s="17">
         <f ca="1">AD7+1</f>
-        <v>45371</v>
+        <v>45373</v>
       </c>
       <c r="AF7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45372</v>
+        <v>45374</v>
       </c>
       <c r="AG7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45373</v>
+        <v>45375</v>
       </c>
       <c r="AH7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45374</v>
+        <v>45376</v>
       </c>
       <c r="AI7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45375</v>
+        <v>45377</v>
       </c>
       <c r="AJ7" s="64">
         <f t="shared" ca="1" si="0"/>
-        <v>45376</v>
+        <v>45378</v>
       </c>
       <c r="AK7" s="17">
         <f ca="1">AJ7+1</f>
-        <v>45377</v>
+        <v>45379</v>
       </c>
       <c r="AL7" s="17">
         <f ca="1">AK7+1</f>
-        <v>45378</v>
+        <v>45380</v>
       </c>
       <c r="AM7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45379</v>
+        <v>45381</v>
       </c>
       <c r="AN7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45380</v>
+        <v>45382</v>
       </c>
       <c r="AO7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45381</v>
+        <v>45383</v>
       </c>
       <c r="AP7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45382</v>
+        <v>45384</v>
       </c>
       <c r="AQ7" s="64">
         <f t="shared" ca="1" si="0"/>
-        <v>45383</v>
+        <v>45385</v>
       </c>
       <c r="AR7" s="17">
         <f ca="1">AQ7+1</f>
-        <v>45384</v>
+        <v>45386</v>
       </c>
       <c r="AS7" s="17">
         <f ca="1">AR7+1</f>
-        <v>45385</v>
+        <v>45387</v>
       </c>
       <c r="AT7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45386</v>
+        <v>45388</v>
       </c>
       <c r="AU7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45387</v>
+        <v>45389</v>
       </c>
       <c r="AV7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45388</v>
+        <v>45390</v>
       </c>
       <c r="AW7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45389</v>
+        <v>45391</v>
       </c>
       <c r="AX7" s="64">
         <f t="shared" ca="1" si="0"/>
-        <v>45390</v>
+        <v>45392</v>
       </c>
       <c r="AY7" s="17">
         <f ca="1">AX7+1</f>
-        <v>45391</v>
+        <v>45393</v>
       </c>
       <c r="AZ7" s="17">
         <f ca="1">AY7+1</f>
-        <v>45392</v>
+        <v>45394</v>
       </c>
       <c r="BA7" s="17">
         <f t="shared" ref="BA7:BE7" ca="1" si="1">AZ7+1</f>
-        <v>45393</v>
+        <v>45395</v>
       </c>
       <c r="BB7" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>45394</v>
+        <v>45396</v>
       </c>
       <c r="BC7" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>45395</v>
+        <v>45397</v>
       </c>
       <c r="BD7" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>45396</v>
+        <v>45398</v>
       </c>
       <c r="BE7" s="64">
         <f t="shared" ca="1" si="1"/>
-        <v>45397</v>
+        <v>45399</v>
       </c>
       <c r="BF7" s="17">
         <f ca="1">BE7+1</f>
-        <v>45398</v>
+        <v>45400</v>
       </c>
       <c r="BG7" s="17">
         <f ca="1">BF7+1</f>
-        <v>45399</v>
+        <v>45401</v>
       </c>
       <c r="BH7" s="17">
         <f t="shared" ref="BH7:BL7" ca="1" si="2">BG7+1</f>
-        <v>45400</v>
+        <v>45402</v>
       </c>
       <c r="BI7" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>45401</v>
+        <v>45403</v>
       </c>
       <c r="BJ7" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>45402</v>
+        <v>45404</v>
       </c>
       <c r="BK7" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>45403</v>
+        <v>45405</v>
       </c>
       <c r="BL7" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>45404</v>
+        <v>45406</v>
       </c>
       <c r="BM7" s="32"/>
     </row>
@@ -10896,23 +10896,23 @@
       </c>
       <c r="J9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="K9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="L9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="M9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="N9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="O9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -10924,23 +10924,23 @@
       </c>
       <c r="Q9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="R9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="S9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="T9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="U9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="V9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -10952,23 +10952,23 @@
       </c>
       <c r="X9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="Y9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="Z9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="AA9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="AB9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="AC9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -10980,23 +10980,23 @@
       </c>
       <c r="AE9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="AF9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="AG9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="AH9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="AI9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="AJ9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -11008,23 +11008,23 @@
       </c>
       <c r="AL9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="AM9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="AN9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="AO9" s="37" t="str">
         <f t="shared" ref="AO9:BL9" ca="1" si="4">LEFT(TEXT(AO7,"TTT"),1)</f>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="AP9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="AQ9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -11036,23 +11036,23 @@
       </c>
       <c r="AS9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="AT9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="AU9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="AV9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="AW9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="AX9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -11064,23 +11064,23 @@
       </c>
       <c r="AZ9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="BA9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="BB9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="BC9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="BD9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="BE9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -11092,23 +11092,23 @@
       </c>
       <c r="BG9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="BH9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="BI9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>S</v>
       </c>
       <c r="BJ9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="BK9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="BL9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -11436,7 +11436,7 @@
       </c>
       <c r="F12" s="23">
         <f ca="1">TODAY()</f>
-        <v>45348</v>
+        <v>45350</v>
       </c>
       <c r="G12" s="24">
         <v>3</v>
@@ -11680,7 +11680,7 @@
       <c r="E13" s="22"/>
       <c r="F13" s="23">
         <f ca="1">TODAY()+5</f>
-        <v>45353</v>
+        <v>45355</v>
       </c>
       <c r="G13" s="24">
         <v>1</v>
@@ -11926,7 +11926,7 @@
       </c>
       <c r="F14" s="23">
         <f ca="1">F12-3</f>
-        <v>45345</v>
+        <v>45347</v>
       </c>
       <c r="G14" s="24">
         <v>10</v>
@@ -12170,7 +12170,7 @@
       <c r="E15" s="22"/>
       <c r="F15" s="23">
         <f ca="1">F12+20</f>
-        <v>45368</v>
+        <v>45370</v>
       </c>
       <c r="G15" s="24">
         <v>1</v>
@@ -12416,7 +12416,7 @@
       </c>
       <c r="F16" s="23">
         <f ca="1">F12+6</f>
-        <v>45354</v>
+        <v>45356</v>
       </c>
       <c r="G16" s="24">
         <v>6</v>
@@ -12899,7 +12899,7 @@
       </c>
       <c r="F18" s="23">
         <f ca="1">F12+6</f>
-        <v>45354</v>
+        <v>45356</v>
       </c>
       <c r="G18" s="24">
         <v>13</v>
@@ -13145,7 +13145,7 @@
       </c>
       <c r="F19" s="23">
         <f ca="1">F18+2</f>
-        <v>45356</v>
+        <v>45358</v>
       </c>
       <c r="G19" s="24">
         <v>9</v>
@@ -13391,7 +13391,7 @@
       </c>
       <c r="F20" s="23">
         <f ca="1">F19+5</f>
-        <v>45361</v>
+        <v>45363</v>
       </c>
       <c r="G20" s="24">
         <v>11</v>
@@ -13635,7 +13635,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="23">
         <f ca="1">F20+2</f>
-        <v>45363</v>
+        <v>45365</v>
       </c>
       <c r="G21" s="24">
         <v>1</v>
@@ -13877,7 +13877,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="23">
         <f ca="1">F21+1</f>
-        <v>45364</v>
+        <v>45366</v>
       </c>
       <c r="G22" s="24">
         <v>24</v>
@@ -14358,7 +14358,7 @@
       <c r="E24" s="22"/>
       <c r="F24" s="23">
         <f ca="1">F12+15</f>
-        <v>45363</v>
+        <v>45365</v>
       </c>
       <c r="G24" s="24">
         <v>4</v>
@@ -14602,7 +14602,7 @@
       <c r="E25" s="22"/>
       <c r="F25" s="23">
         <f ca="1">F24+3</f>
-        <v>45366</v>
+        <v>45368</v>
       </c>
       <c r="G25" s="24">
         <v>14</v>
@@ -14846,7 +14846,7 @@
       <c r="E26" s="22"/>
       <c r="F26" s="23">
         <f ca="1">F25+15</f>
-        <v>45381</v>
+        <v>45383</v>
       </c>
       <c r="G26" s="24">
         <v>6</v>
@@ -15090,7 +15090,7 @@
       <c r="E27" s="22"/>
       <c r="F27" s="23">
         <f ca="1">F21+22</f>
-        <v>45385</v>
+        <v>45387</v>
       </c>
       <c r="G27" s="24">
         <v>3</v>
@@ -15334,7 +15334,7 @@
       <c r="E28" s="22"/>
       <c r="F28" s="23">
         <f ca="1">F16</f>
-        <v>45354</v>
+        <v>45356</v>
       </c>
       <c r="G28" s="24">
         <v>19</v>
@@ -15813,7 +15813,7 @@
       <c r="E30" s="22"/>
       <c r="F30" s="23">
         <f ca="1">F27+3</f>
-        <v>45388</v>
+        <v>45390</v>
       </c>
       <c r="G30" s="24">
         <v>15</v>
@@ -16055,7 +16055,7 @@
       <c r="E31" s="22"/>
       <c r="F31" s="23">
         <f ca="1">F30+14</f>
-        <v>45402</v>
+        <v>45404</v>
       </c>
       <c r="G31" s="24">
         <v>5</v>
@@ -16299,7 +16299,7 @@
       <c r="E32" s="22"/>
       <c r="F32" s="23">
         <f ca="1">F31+42</f>
-        <v>45444</v>
+        <v>45446</v>
       </c>
       <c r="G32" s="24">
         <v>1</v>
@@ -17478,8 +17478,8 @@
   </sheetPr>
   <dimension ref="A1:JE49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -41534,7 +41534,7 @@
       </c>
       <c r="D37" s="59"/>
       <c r="E37" s="60">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="F37" s="61">
         <v>45209</v>
@@ -42581,7 +42581,7 @@
       </c>
       <c r="D38" s="59"/>
       <c r="E38" s="60">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F38" s="61">
         <v>45217</v>
@@ -43628,7 +43628,7 @@
       </c>
       <c r="D39" s="59"/>
       <c r="E39" s="60">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F39" s="61">
         <v>45225</v>
@@ -49879,7 +49879,7 @@
       <c r="D45" s="59"/>
       <c r="E45" s="60">
         <f xml:space="preserve"> (E12+E13+E14+E18+E19+E20+E25+E26+E27+E30+E37+E38+E39+E40+E41)/15</f>
-        <v>0.41333333333333327</v>
+        <v>0.49999999999999994</v>
       </c>
       <c r="F45" s="61"/>
       <c r="G45" s="62"/>
@@ -55558,15 +55558,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -55584,6 +55575,15 @@
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55608,14 +55608,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAF2F40C-D12E-4644-AA6E-31E499F048DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CD6AD73-D703-40CF-AB8D-72E6A3921BEB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -55625,4 +55617,12 @@
     <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAF2F40C-D12E-4644-AA6E-31E499F048DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>